<commit_message>
Using Pandas to load csv, xls and xlsx data.
</commit_message>
<xml_diff>
--- a/data/Main_Phases_of_Flight/main_phases_of_flight.xlsx
+++ b/data/Main_Phases_of_Flight/main_phases_of_flight.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Loyd IV\AppData\Local\Microsoft\Windows\INetCache\Content.Outlook\0QPDZ33X\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SoftDevelopment\Projects\IO-Aero\io-avstats\data\Main_Phases_of_Flight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35F2B52B-9624-4A8E-B7D6-7CDE73D65912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29797B4-BCDB-4090-8B09-81EBD51B4AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30000" yWindow="465" windowWidth="27315" windowHeight="14925" xr2:uid="{2834C7AD-6633-452B-A344-36B621245E70}"/>
+    <workbookView xWindow="3040" yWindow="0" windowWidth="25780" windowHeight="20880" xr2:uid="{2834C7AD-6633-452B-A344-36B621245E70}"/>
   </bookViews>
   <sheets>
-    <sheet name="io_md_codes_phase_202304062020_" sheetId="2" r:id="rId1"/>
+    <sheet name="io_md_codes_phase" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">io_md_codes_phase_202304062020_!$A$1:$B$49</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">io_md_codes_phase!$A$1:$B$49</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -583,18 +583,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFD8099-4BC7-4D4B-A459-92FEA85884AA}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -605,7 +605,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>100</v>
       </c>
@@ -616,7 +616,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>150</v>
       </c>
@@ -627,7 +627,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>151</v>
       </c>
@@ -638,7 +638,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>152</v>
       </c>
@@ -649,7 +649,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>153</v>
       </c>
@@ -660,7 +660,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>154</v>
       </c>
@@ -671,7 +671,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>200</v>
       </c>
@@ -682,7 +682,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>201</v>
       </c>
@@ -693,7 +693,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>202</v>
       </c>
@@ -704,7 +704,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>203</v>
       </c>
@@ -715,7 +715,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>250</v>
       </c>
@@ -726,7 +726,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>251</v>
       </c>
@@ -737,7 +737,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>252</v>
       </c>
@@ -748,7 +748,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>253</v>
       </c>
@@ -759,7 +759,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>300</v>
       </c>
@@ -770,7 +770,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>301</v>
       </c>
@@ -781,7 +781,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>350</v>
       </c>
@@ -792,7 +792,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>400</v>
       </c>
@@ -803,7 +803,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>401</v>
       </c>
@@ -814,7 +814,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>402</v>
       </c>
@@ -825,7 +825,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>403</v>
       </c>
@@ -836,7 +836,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>404</v>
       </c>
@@ -847,7 +847,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>405</v>
       </c>
@@ -858,7 +858,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>450</v>
       </c>
@@ -869,7 +869,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>451</v>
       </c>
@@ -880,7 +880,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>452</v>
       </c>
@@ -891,7 +891,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>453</v>
       </c>
@@ -902,7 +902,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>500</v>
       </c>
@@ -913,7 +913,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>501</v>
       </c>
@@ -924,7 +924,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>502</v>
       </c>
@@ -935,7 +935,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>503</v>
       </c>
@@ -946,7 +946,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>504</v>
       </c>
@@ -957,7 +957,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>505</v>
       </c>
@@ -968,7 +968,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>506</v>
       </c>
@@ -979,7 +979,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>507</v>
       </c>
@@ -990,7 +990,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>508</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>509</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>550</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>551</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>552</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>553</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>600</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>601</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>650</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>700</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>750</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>800</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>990</v>
       </c>
@@ -1147,7 +1147,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>